<commit_message>
terminando o classificador do dataset
</commit_message>
<xml_diff>
--- a/olympics.xlsx
+++ b/olympics.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22704"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B39A975-87D7-403C-9AA6-B0B190DCDD4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B2DE313-2A06-4F98-8C8C-5C3F8603BDBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="603">
   <si>
     <t>Treinamento</t>
   </si>
@@ -2133,176 +2133,6 @@
 #tokyo2020
 #coronavirus
 https://t.co/ophzzqf6ng</t>
-  </si>
-  <si>
-    <t>rt @toisports: #breaking #olympicqualifiers #tokyo2020
-@lovlinaborgohai loses 0-5 to hong gu of china in women's 69kg semifinals
-she had…</t>
-  </si>
-  <si>
-    <t>rt @rick_eichhornr: 3rd islamic wave -- september 11, 2001, eu migrant invasion continues
-just prior: airline hijackings, munich olympics m…</t>
-  </si>
-  <si>
-    <t>going to be really interesting to see how they restructure after this. also, if the olympics were to be rescheduled (more likely to be cancelled) they’d probably take place in october, which is where they moved the g1. https://t.co/bf8bk8akci</t>
-  </si>
-  <si>
-    <t>greece’s olympic committee announced monday that no spectators will be allowed at the tokyo 2020 olympics torch lighting ceremony in ancient olympia on thursday due to the coronavirus outbreak.
-#coronavirus</t>
-  </si>
-  <si>
-    <t>@jamiec1979 @pe_mme @lisanandy also trans people have been allowed to compete in the olympics since 2004, none have ever won a gold medal. in fact not one has even made it to the the olympics. you are making an issue of something that hardly exists .</t>
-  </si>
-  <si>
-    <t>kill the olympics. https://t.co/pjwoqeqxxc</t>
-  </si>
-  <si>
-    <t>@clairlemon not japan. they have an olympics to host in a few months so everyone relax its all totally ok here 🙃</t>
-  </si>
-  <si>
-    <t>rt @sherni02: #اسلام_کی_شہزادياں 
-minhal sohail the 21-year-old became pakistan’s first female shooter to compete at olympics 2016. althoug…</t>
-  </si>
-  <si>
-    <t>rt @billsimmons: unnerving state of play as the coronavirus interferes in everyday life - by brian phillips  https://t.co/otkwjrdr8j</t>
-  </si>
-  <si>
-    <t>@fancypirate8 i love the olympics.  cool to see these incredible athletes</t>
-  </si>
-  <si>
-    <t>rt @reuters: japan's 2011 fukushima nuclear disaster marked a turning point for this father and son: for one it was the end of the life he…</t>
-  </si>
-  <si>
-    <t>with all the sickness fears, will tokyo run the olympics this year? https://t.co/11kcuqttqs https://t.co/4kabgsgcte</t>
-  </si>
-  <si>
-    <t>rt @lisacullen: in #japan, the following are closed due to #coronavirus:
-✘ all schools
-✘ many offices
-✘ disneyland
-✘ baseball, sumo, al…</t>
-  </si>
-  <si>
-    <t>rt @abscbnnews: olympics: pinoy athletes continue to vie for slots despite possible postponement of tokyo games https://t.co/xidjghvnym</t>
-  </si>
-  <si>
-    <t>with the format of the olympics this year i have no issue with team selection being too 4 aa at trials!</t>
-  </si>
-  <si>
-    <t>@lisanandy what a wet fish you were on tv this morning. no leadership credentials for you. men running in emailing olympics needs a committee to decide if it's right? not common sensecprevailing your side</t>
-  </si>
-  <si>
-    <t>@sacrasmnazi @clelyly yes first round is tricky, but i am only worried about first round . because my gut says she'll swallow okuhara and ratchanok , although it'll be tough to swallow ratchanok a good potenial quarterfianals seems to bring saina close towards her fourth consecutive olympics</t>
-  </si>
-  <si>
-    <t>rt @newday: japan’s infection rate is under scrutiny as coronavirus casts a shadow over the upcoming summer olympics.
-“japanese epidemiolog…</t>
-  </si>
-  <si>
-    <t>@pgtitour @tokyo2020 @olympics @chikkarangappa @naam5 @gangjeer @virajmadappa @tatasteelltd tee-off is 11th or 12th? thx.</t>
-  </si>
-  <si>
-    <t>rt @sportsdeskph: the tokyo 2020 olympic torch lighting ceremony at the site of ancient olympia will be staged without spectators on thursd…</t>
-  </si>
-  <si>
-    <t>sometimes the real subject of a story isn't the one you expected. 
-after fukushima, a young baseball star triumphed. but the one i cared most about in this story was the father, who lost everything he knew.
-as always, loved working with @saitomri on this.
-https://t.co/urzsy6nkyt https://t.co/adtkx5ixx4</t>
-  </si>
-  <si>
-    <t>rt @truthabtchina: the 2022 winter olympics should not be held in china. the world should not support the ccp with their terrible human rig…</t>
-  </si>
-  <si>
-    <t>rt @bbcsportwales: 🚣‍♀️ @vickythornleygb is aiming to make her third olympics this year. 
-after a silver in the double sculls at rio she's…</t>
-  </si>
-  <si>
-    <t>rt @itgdsports: having sealed tokyo olympics berths, amit panghal and lovlina borgohain finished the asian qualifiers with bronze medals |…</t>
-  </si>
-  <si>
-    <t>rt @tokyo2020: the boxing is back on! 🥊
-watch the qualifiers live from amman right here: 
-https://t.co/jierrhrksq
-#boxing #roadtotokyo20…</t>
-  </si>
-  <si>
-    <t>@mattbakerfans @bbccountryfile @bbcone @olympics @nestle @rspca_official @missalexjones @cbbc can you help?!??</t>
-  </si>
-  <si>
-    <t>nesthy petecio rues failed first shot at tokyo olympics - https://t.co/jonrdawmbu https://t.co/qbig9xiseh</t>
-  </si>
-  <si>
-    <t>rt @kevin10tv: fans barred from tokyo 2020 torch ceremony - via @espn app https://t.co/8yjt5q75wl</t>
-  </si>
-  <si>
-    <t>rt @sentandent: the tentacles of canceling the tokyo olympics — or postponing or staging it in empty venues — would reach into every corner…</t>
-  </si>
-  <si>
-    <t>rt @joebrentmando: if you wanted to time a global pandemic for maximum effect, you’d put it in the middle of an olympics and an american el…</t>
-  </si>
-  <si>
-    <t>@ibnabitareq @saajidlipham sorry, tareq. i won’t drink your liberal kool aid. let’s not play the liberal olympics. haram is haram. say it with your chest. homosexuality is forbidden in islam. are you afraid to lose followers?</t>
-  </si>
-  <si>
-    <t>the impact of olympic cancellation would reach around the globe https://t.co/kkl5azmpof https://t.co/tf63wqnbh5</t>
-  </si>
-  <si>
-    <t>rt @staronline: indonesia considers 2032 olympics bid for new capital city with softbank's help
-https://t.co/he1r7dpqnx  https://t.co/he1r7…</t>
-  </si>
-  <si>
-    <t>the nsas must figure out how their athletes can participate in their respective #tokyo2020 olympics qualifiers https://t.co/6uvjo7yjae via @rapplerdotcom</t>
-  </si>
-  <si>
-    <t>@thefifth_wave forgot about the olympics 😂</t>
-  </si>
-  <si>
-    <t>rt @reuters: #tokyo2020 baseball and softball games will be held in fukushima, which suffered nuclear meltdowns in 2011. organizers hope th…</t>
-  </si>
-  <si>
-    <t>rt @alexshibutani: last night was a dream that became a reality. @maiashibutani and i have worked so hard for this! proud to be the first i…</t>
-  </si>
-  <si>
-    <t>exclusive: indonesia considers 2032 olympics bid for new capital city with softbank's help https://t.co/q4c8yd7hmf</t>
-  </si>
-  <si>
-    <t>ambitious! #indonesian president joko widodo is weighing an audacious 2032 #olympics bid centered on the country's not-yet-built new capital and is in early talks with #softbank and other investors for support(reuters) https://t.co/zhgmdia3gn</t>
-  </si>
-  <si>
-    <t>rt @cityofpomo: congratulations to reid and fiona who brought home a total of 7 medals from the 2020 special olympics canadian winter games…</t>
-  </si>
-  <si>
-    <t>the future is uncertain and impossible to forecast. we do not try, preferring to follow a process with c.150yrs of data that shows that buying businesses for less than their intrinsic value will, on average and over time, yield above-average returns.
-https://t.co/ncljojzdxj</t>
-  </si>
-  <si>
-    <t>there isn't one insurer that holds all the risk for the cancellation of a major event like the olympics or a world cup. the main counterparty would typically parcel out its own risk to several other so the pain can be shared.</t>
-  </si>
-  <si>
-    <t>from the special issue: japan’s olympic summer games - past &amp;amp; present. this article comes from the section of branding and identity.  
-opening a storyline in the 2020 olympics
-by @david_leheny
-https://t.co/wrl1jxdeh2 
-#tokyoolympics @japan_olympic https://t.co/9veswjb4sz</t>
-  </si>
-  <si>
-    <t>@lincolnfresno gender determination in athletics, a century old question/problem has worked its way down to middle school events and daily life.  1936 olympics to '68 to 2020.
-https://t.co/rmkretdwqi https://t.co/a1ussyvi80</t>
-  </si>
-  <si>
-    <t>if only snowy had fortified himself at the 1908 london olympics when boxing against (then future) english cricket captain jwht douglas he might have secured a gold medal, instead of the silver... https://t.co/urlcxpcnrz https://t.co/mk5nn1n13o</t>
-  </si>
-  <si>
-    <t>rt @clintoncity_ccs: check out wbir’s coverage of our blaze special olympics!   https://t.co/73psqjjjc9</t>
-  </si>
-  <si>
-    <t>rt @toisports: #justin #olympicqualifiers #tokyo2020 #boxing
-@boxerpanghal loses to jianguan hu of china in 52kg semis
-amit had already q…</t>
-  </si>
-  <si>
-    <t>rt @eggiebabie: making fun of someone’s height is still body shaming and it doesn’t matter which one is inherently “worst” because it isn’t…</t>
   </si>
 </sst>
 </file>
@@ -2706,8 +2536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="B251" sqref="B251"/>
+    <sheetView topLeftCell="A392" workbookViewId="0">
+      <selection activeCell="B502" sqref="B502"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4720,1255 +4550,2008 @@
       <c r="A251" t="s">
         <v>251</v>
       </c>
+      <c r="B251">
+        <v>0</v>
+      </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252" t="s">
         <v>252</v>
       </c>
+      <c r="B252">
+        <v>0</v>
+      </c>
     </row>
     <row r="253" spans="1:2">
       <c r="A253" t="s">
         <v>253</v>
       </c>
+      <c r="B253">
+        <v>0</v>
+      </c>
     </row>
     <row r="254" spans="1:2">
       <c r="A254" t="s">
         <v>254</v>
       </c>
+      <c r="B254">
+        <v>0</v>
+      </c>
     </row>
     <row r="255" spans="1:2">
       <c r="A255" t="s">
         <v>255</v>
       </c>
+      <c r="B255">
+        <v>0</v>
+      </c>
     </row>
     <row r="256" spans="1:2">
       <c r="A256" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="257" spans="1:1">
+      <c r="B256">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2">
       <c r="A257" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="258" spans="1:1">
+      <c r="B257">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2">
       <c r="A258" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="259" spans="1:1">
+      <c r="B258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2">
       <c r="A259" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="260" spans="1:1">
+      <c r="B259">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2">
       <c r="A260" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="261" spans="1:1">
+      <c r="B260">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2">
       <c r="A261" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="262" spans="1:1">
+      <c r="B261">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2">
       <c r="A262" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="263" spans="1:1">
+      <c r="B262">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2">
       <c r="A263" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="264" spans="1:1">
+      <c r="B263">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2">
       <c r="A264" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="265" spans="1:1">
+      <c r="B264">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2">
       <c r="A265" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="266" spans="1:1">
+      <c r="B265">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2">
       <c r="A266" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="267" spans="1:1">
+      <c r="B266">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2">
       <c r="A267" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="268" spans="1:1">
+      <c r="B267">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2">
       <c r="A268" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="269" spans="1:1">
+      <c r="B268">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2">
       <c r="A269" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="270" spans="1:1">
+      <c r="B269">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2">
       <c r="A270" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="271" spans="1:1">
+      <c r="B270">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2">
       <c r="A271" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="272" spans="1:1">
+      <c r="B271">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2">
       <c r="A272" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="273" spans="1:1">
+      <c r="B272">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2">
       <c r="A273" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="274" spans="1:1">
+      <c r="B273">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2">
       <c r="A274" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="275" spans="1:1">
+      <c r="B274">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2">
       <c r="A275" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="276" spans="1:1">
+      <c r="B275">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2">
       <c r="A276" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="277" spans="1:1">
+      <c r="B276">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2">
       <c r="A277" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="278" spans="1:1">
+      <c r="B277">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2">
       <c r="A278" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="279" spans="1:1">
+      <c r="B278">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2">
       <c r="A279" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="280" spans="1:1">
+      <c r="B279">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2">
       <c r="A280" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="281" spans="1:1">
+      <c r="B280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2">
       <c r="A281" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="282" spans="1:1">
+      <c r="B281">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2">
       <c r="A282" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="283" spans="1:1">
+      <c r="B282">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2">
       <c r="A283" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="284" spans="1:1">
+      <c r="B283">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2">
       <c r="A284" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="285" spans="1:1">
+      <c r="B284">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2">
       <c r="A285" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="286" spans="1:1">
+      <c r="B285">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2">
       <c r="A286" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="287" spans="1:1">
+      <c r="B286">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2">
       <c r="A287" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="288" spans="1:1">
+      <c r="B287">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2">
       <c r="A288" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="289" spans="1:1">
+      <c r="B288">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2">
       <c r="A289" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="290" spans="1:1">
+      <c r="B289">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2">
       <c r="A290" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="291" spans="1:1">
+      <c r="B290">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2">
       <c r="A291" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="292" spans="1:1">
+      <c r="B291">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2">
       <c r="A292" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="293" spans="1:1">
+      <c r="B292">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2">
       <c r="A293" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="294" spans="1:1">
+      <c r="B293">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2">
       <c r="A294" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="295" spans="1:1">
+      <c r="B294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2">
       <c r="A295" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="296" spans="1:1">
+      <c r="B295">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2">
       <c r="A296" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="297" spans="1:1">
+      <c r="B296">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2">
       <c r="A297" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="298" spans="1:1">
+      <c r="B297">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2">
       <c r="A298" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="299" spans="1:1">
+      <c r="B298">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2">
       <c r="A299" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="300" spans="1:1">
+      <c r="B299">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2">
       <c r="A300" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="301" spans="1:1">
+      <c r="B300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2">
       <c r="A301" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="302" spans="1:1">
+      <c r="B301">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2">
       <c r="A302" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="303" spans="1:1">
+      <c r="B302">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2">
       <c r="A303" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="304" spans="1:1">
+      <c r="B303">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2">
       <c r="A304" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="305" spans="1:1">
+      <c r="B304">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2">
       <c r="A305" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="306" spans="1:1">
+      <c r="B305">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2">
       <c r="A306" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="307" spans="1:1">
+      <c r="B306">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2">
       <c r="A307" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="308" spans="1:1">
+      <c r="B307">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2">
       <c r="A308" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="309" spans="1:1">
+      <c r="B308">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2">
       <c r="A309" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="310" spans="1:1">
+      <c r="B309">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2">
       <c r="A310" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="311" spans="1:1">
+      <c r="B310">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2">
       <c r="A311" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="312" spans="1:1">
+      <c r="B311">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2">
       <c r="A312" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="313" spans="1:1">
+      <c r="B312">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2">
       <c r="A313" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="314" spans="1:1">
+      <c r="B313">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2">
       <c r="A314" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="315" spans="1:1">
+      <c r="B314">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2">
       <c r="A315" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="316" spans="1:1">
+      <c r="B315">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2">
       <c r="A316" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="317" spans="1:1">
+      <c r="B316">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2">
       <c r="A317" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="318" spans="1:1">
+      <c r="B317">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2">
       <c r="A318" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="319" spans="1:1">
+      <c r="B318">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2">
       <c r="A319" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="320" spans="1:1">
+      <c r="B319">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2">
       <c r="A320" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="321" spans="1:1">
+      <c r="B320">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2">
       <c r="A321" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="322" spans="1:1">
+      <c r="B321">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2">
       <c r="A322" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="323" spans="1:1">
+      <c r="B322">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2">
       <c r="A323" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="324" spans="1:1">
+      <c r="B323">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2">
       <c r="A324" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="325" spans="1:1">
+      <c r="B324">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2">
       <c r="A325" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="326" spans="1:1">
+      <c r="B325">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2">
       <c r="A326" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="327" spans="1:1">
+      <c r="B326">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2">
       <c r="A327" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="328" spans="1:1">
+      <c r="B327">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2">
       <c r="A328" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="329" spans="1:1">
+      <c r="B328">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2">
       <c r="A329" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="330" spans="1:1">
+      <c r="B329">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2">
       <c r="A330" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="331" spans="1:1">
+      <c r="B330">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2">
       <c r="A331" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="332" spans="1:1">
+      <c r="B331">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2">
       <c r="A332" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="333" spans="1:1">
+      <c r="B332">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2">
       <c r="A333" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="334" spans="1:1">
+      <c r="B333">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2">
       <c r="A334" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="335" spans="1:1">
+      <c r="B334">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2">
       <c r="A335" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="336" spans="1:1">
+      <c r="B335">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2">
       <c r="A336" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="337" spans="1:1">
+      <c r="B336">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2">
       <c r="A337" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="338" spans="1:1">
+      <c r="B337">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2">
       <c r="A338" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="339" spans="1:1">
+      <c r="B338">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2">
       <c r="A339" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="340" spans="1:1">
+      <c r="B339">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2">
       <c r="A340" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="341" spans="1:1">
+      <c r="B340">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2">
       <c r="A341" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="342" spans="1:1">
+      <c r="B341">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2">
       <c r="A342" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="343" spans="1:1">
+      <c r="B342">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2">
       <c r="A343" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="344" spans="1:1">
+      <c r="B343">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2">
       <c r="A344" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="345" spans="1:1">
+      <c r="B344">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2">
       <c r="A345" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="346" spans="1:1">
+      <c r="B345">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2">
       <c r="A346" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="347" spans="1:1">
+      <c r="B346">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2">
       <c r="A347" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="348" spans="1:1">
+      <c r="B347">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2">
       <c r="A348" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="349" spans="1:1">
+      <c r="B348">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2">
       <c r="A349" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="350" spans="1:1">
+      <c r="B349">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2">
       <c r="A350" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="351" spans="1:1">
+      <c r="B350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2">
       <c r="A351" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="352" spans="1:1">
+      <c r="B351">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2">
       <c r="A352" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="353" spans="1:1">
+      <c r="B352">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2">
       <c r="A353" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="354" spans="1:1">
+      <c r="B353">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2">
       <c r="A354" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="355" spans="1:1">
+      <c r="B354">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2">
       <c r="A355" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="356" spans="1:1">
+      <c r="B355">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2">
       <c r="A356" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="357" spans="1:1">
+      <c r="B356">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2">
       <c r="A357" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="358" spans="1:1">
+      <c r="B357">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2">
       <c r="A358" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="359" spans="1:1">
+      <c r="B358">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2">
       <c r="A359" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="360" spans="1:1">
+      <c r="B359">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2">
       <c r="A360" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="361" spans="1:1">
+      <c r="B360">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2">
       <c r="A361" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="362" spans="1:1">
+      <c r="B361">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2">
       <c r="A362" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="363" spans="1:1">
+      <c r="B362">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2">
       <c r="A363" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="364" spans="1:1">
+      <c r="B363">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2">
       <c r="A364" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="365" spans="1:1">
+      <c r="B364">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2">
       <c r="A365" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="366" spans="1:1">
+      <c r="B365">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2">
       <c r="A366" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="367" spans="1:1">
+      <c r="B366">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2">
       <c r="A367" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="368" spans="1:1">
+      <c r="B367">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2">
       <c r="A368" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="369" spans="1:1">
+      <c r="B368">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2">
       <c r="A369" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="370" spans="1:1">
+      <c r="B369">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2">
       <c r="A370" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="371" spans="1:1">
+      <c r="B370">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2">
       <c r="A371" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="372" spans="1:1">
+      <c r="B371">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2">
       <c r="A372" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="373" spans="1:1">
+      <c r="B372">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2">
       <c r="A373" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="374" spans="1:1">
+      <c r="B373">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2">
       <c r="A374" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="375" spans="1:1">
+      <c r="B374">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2">
       <c r="A375" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="376" spans="1:1">
+      <c r="B375">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2">
       <c r="A376" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="377" spans="1:1">
+      <c r="B376">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2">
       <c r="A377" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="378" spans="1:1">
+      <c r="B377">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2">
       <c r="A378" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="379" spans="1:1">
+      <c r="B378">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2">
       <c r="A379" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="380" spans="1:1">
+      <c r="B379">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2">
       <c r="A380" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="381" spans="1:1">
+      <c r="B380">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2">
       <c r="A381" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="382" spans="1:1">
+      <c r="B381">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2">
       <c r="A382" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="383" spans="1:1">
+      <c r="B382">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2">
       <c r="A383" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="384" spans="1:1">
+      <c r="B383">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2">
       <c r="A384" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="385" spans="1:1">
+      <c r="B384">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2">
       <c r="A385" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="386" spans="1:1">
+      <c r="B385">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2">
       <c r="A386" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="387" spans="1:1">
+      <c r="B386">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2">
       <c r="A387" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="388" spans="1:1">
+      <c r="B387">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2">
       <c r="A388" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="389" spans="1:1">
+      <c r="B388">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2">
       <c r="A389" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="390" spans="1:1">
+      <c r="B389">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2">
       <c r="A390" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="391" spans="1:1">
+      <c r="B390">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2">
       <c r="A391" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="392" spans="1:1">
+      <c r="B391">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2">
       <c r="A392" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="393" spans="1:1">
+      <c r="B392">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2">
       <c r="A393" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="394" spans="1:1">
+      <c r="B393">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2">
       <c r="A394" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="395" spans="1:1">
+      <c r="B394">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2">
       <c r="A395" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="396" spans="1:1">
+      <c r="B395">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2">
       <c r="A396" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="397" spans="1:1">
+      <c r="B396">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2">
       <c r="A397" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="398" spans="1:1">
+      <c r="B397">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2">
       <c r="A398" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="399" spans="1:1">
+      <c r="B398">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2">
       <c r="A399" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="400" spans="1:1">
+      <c r="B399">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2">
       <c r="A400" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="401" spans="1:1">
+      <c r="B400">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2">
       <c r="A401" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="402" spans="1:1">
+      <c r="B401">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2">
       <c r="A402" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="403" spans="1:1">
+      <c r="B402">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2">
       <c r="A403" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="404" spans="1:1">
+      <c r="B403">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2">
       <c r="A404" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="405" spans="1:1">
+      <c r="B404">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2">
       <c r="A405" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="406" spans="1:1">
+      <c r="B405">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2">
       <c r="A406" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="407" spans="1:1">
+      <c r="B406">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2">
       <c r="A407" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="408" spans="1:1">
+      <c r="B407">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2">
       <c r="A408" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="409" spans="1:1">
+      <c r="B408">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2">
       <c r="A409" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="410" spans="1:1">
+      <c r="B409">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2">
       <c r="A410" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="411" spans="1:1">
+      <c r="B410">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2">
       <c r="A411" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="412" spans="1:1">
+      <c r="B411">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2">
       <c r="A412" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="413" spans="1:1">
+      <c r="B412">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2">
       <c r="A413" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="414" spans="1:1">
+      <c r="B413">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2">
       <c r="A414" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="415" spans="1:1">
+      <c r="B414">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2">
       <c r="A415" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="416" spans="1:1">
+      <c r="B415">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2">
       <c r="A416" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="417" spans="1:1">
+      <c r="B416">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2">
       <c r="A417" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="418" spans="1:1">
+      <c r="B417">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2">
       <c r="A418" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="419" spans="1:1">
+      <c r="B418">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2">
       <c r="A419" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="420" spans="1:1">
+      <c r="B419">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2">
       <c r="A420" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="421" spans="1:1">
+      <c r="B420">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2">
       <c r="A421" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="422" spans="1:1">
+      <c r="B421">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2">
       <c r="A422" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="423" spans="1:1">
+      <c r="B422">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2">
       <c r="A423" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="424" spans="1:1">
+      <c r="B423">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2">
       <c r="A424" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="425" spans="1:1">
+      <c r="B424">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2">
       <c r="A425" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="426" spans="1:1">
+      <c r="B425">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2">
       <c r="A426" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="427" spans="1:1">
+      <c r="B426">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2">
       <c r="A427" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="428" spans="1:1">
+      <c r="B427">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2">
       <c r="A428" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="429" spans="1:1">
+      <c r="B428">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="429" spans="1:2">
       <c r="A429" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="430" spans="1:1">
+      <c r="B429">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="430" spans="1:2">
       <c r="A430" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="431" spans="1:1">
+      <c r="B430">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2">
       <c r="A431" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="432" spans="1:1">
+      <c r="B431">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2">
       <c r="A432" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="433" spans="1:1">
+      <c r="B432">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2">
       <c r="A433" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="434" spans="1:1">
+      <c r="B433">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2">
       <c r="A434" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="435" spans="1:1">
+      <c r="B434">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2">
       <c r="A435" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="436" spans="1:1">
+      <c r="B435">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2">
       <c r="A436" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="437" spans="1:1">
+      <c r="B436">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2">
       <c r="A437" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="438" spans="1:1">
+      <c r="B437">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2">
       <c r="A438" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="439" spans="1:1">
+      <c r="B438">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2">
       <c r="A439" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="440" spans="1:1">
+      <c r="B439">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2">
       <c r="A440" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="441" spans="1:1">
+      <c r="B440">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2">
       <c r="A441" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="442" spans="1:1">
+      <c r="B441">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2">
       <c r="A442" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="443" spans="1:1">
+      <c r="B442">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2">
       <c r="A443" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="444" spans="1:1">
+      <c r="B443">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2">
       <c r="A444" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="445" spans="1:1">
+      <c r="B444">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2">
       <c r="A445" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="446" spans="1:1">
+      <c r="B445">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2">
       <c r="A446" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="447" spans="1:1">
+      <c r="B446">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="447" spans="1:2">
       <c r="A447" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="448" spans="1:1">
+      <c r="B447">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2">
       <c r="A448" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="449" spans="1:1">
+      <c r="B448">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2">
       <c r="A449" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="450" spans="1:1">
+      <c r="B449">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="450" spans="1:2">
       <c r="A450" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="451" spans="1:1">
+      <c r="B450">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2">
       <c r="A451" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="452" spans="1:1">
+      <c r="B451">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2">
       <c r="A452" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="453" spans="1:1">
+      <c r="B452">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="453" spans="1:2">
       <c r="A453" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="454" spans="1:1">
+      <c r="B453">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="454" spans="1:2">
       <c r="A454" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="455" spans="1:1">
+      <c r="B454">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2">
       <c r="A455" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="456" spans="1:1">
+      <c r="B455">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="456" spans="1:2">
       <c r="A456" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="457" spans="1:1">
+      <c r="B456">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="457" spans="1:2">
       <c r="A457" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="458" spans="1:1">
+      <c r="B457">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="458" spans="1:2">
       <c r="A458" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="459" spans="1:1">
+      <c r="B458">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2">
       <c r="A459" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="460" spans="1:1">
+      <c r="B459">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="460" spans="1:2">
       <c r="A460" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="461" spans="1:1">
+      <c r="B460">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="461" spans="1:2">
       <c r="A461" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="462" spans="1:1">
+      <c r="B461">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="462" spans="1:2">
       <c r="A462" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="463" spans="1:1">
+      <c r="B462">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="463" spans="1:2">
       <c r="A463" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="464" spans="1:1">
+      <c r="B463">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="464" spans="1:2">
       <c r="A464" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="465" spans="1:1">
+      <c r="B464">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2">
       <c r="A465" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="466" spans="1:1">
+      <c r="B465">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="466" spans="1:2">
       <c r="A466" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="467" spans="1:1">
+      <c r="B466">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2">
       <c r="A467" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="468" spans="1:1">
+      <c r="B467">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2">
       <c r="A468" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="469" spans="1:1">
+      <c r="B468">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="469" spans="1:2">
       <c r="A469" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="470" spans="1:1">
+      <c r="B469">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2">
       <c r="A470" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="471" spans="1:1">
+      <c r="B470">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="471" spans="1:2">
       <c r="A471" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="472" spans="1:1">
+      <c r="B471">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2">
       <c r="A472" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="473" spans="1:1">
+      <c r="B472">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2">
       <c r="A473" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="474" spans="1:1">
+      <c r="B473">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2">
       <c r="A474" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="475" spans="1:1">
+      <c r="B474">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2">
       <c r="A475" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="476" spans="1:1">
+      <c r="B475">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2">
       <c r="A476" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="477" spans="1:1">
+      <c r="B476">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="477" spans="1:2">
       <c r="A477" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="478" spans="1:1">
+      <c r="B477">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2">
       <c r="A478" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="479" spans="1:1">
+      <c r="B478">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2">
       <c r="A479" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="480" spans="1:1">
+      <c r="B479">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2">
       <c r="A480" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="481" spans="1:1">
+      <c r="B480">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="481" spans="1:2">
       <c r="A481" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="482" spans="1:1">
+      <c r="B481">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="482" spans="1:2">
       <c r="A482" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="483" spans="1:1">
+      <c r="B482">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="483" spans="1:2">
       <c r="A483" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="484" spans="1:1">
+      <c r="B483">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="484" spans="1:2">
       <c r="A484" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="485" spans="1:1">
+      <c r="B484">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="485" spans="1:2">
       <c r="A485" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="486" spans="1:1">
+      <c r="B485">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="486" spans="1:2">
       <c r="A486" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="487" spans="1:1">
+      <c r="B486">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="487" spans="1:2">
       <c r="A487" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="488" spans="1:1">
+      <c r="B487">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="488" spans="1:2">
       <c r="A488" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="489" spans="1:1">
+      <c r="B488">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="489" spans="1:2">
       <c r="A489" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="490" spans="1:1">
+      <c r="B489">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="490" spans="1:2">
       <c r="A490" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="491" spans="1:1">
+      <c r="B490">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="491" spans="1:2">
       <c r="A491" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="492" spans="1:1">
+      <c r="B491">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="492" spans="1:2">
       <c r="A492" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="493" spans="1:1">
+      <c r="B492">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="493" spans="1:2">
       <c r="A493" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="494" spans="1:1">
+      <c r="B493">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="494" spans="1:2">
       <c r="A494" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="495" spans="1:1">
+      <c r="B494">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="495" spans="1:2">
       <c r="A495" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="496" spans="1:1">
+      <c r="B495">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="496" spans="1:2">
       <c r="A496" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="497" spans="1:1">
+      <c r="B496">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="497" spans="1:2">
       <c r="A497" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="498" spans="1:1">
+      <c r="B497">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="498" spans="1:2">
       <c r="A498" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="499" spans="1:1">
+      <c r="B498">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="499" spans="1:2">
       <c r="A499" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="500" spans="1:1">
+      <c r="B499">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="500" spans="1:2">
       <c r="A500" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="501" spans="1:1">
+      <c r="B500">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="501" spans="1:2">
       <c r="A501" t="s">
         <v>501</v>
+      </c>
+      <c r="B501">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5978,758 +6561,824 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A149"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="B28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="B38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="B39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
+      <c r="B40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="42" spans="1:1">
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="43" spans="1:1">
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="44" spans="1:1">
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="45" spans="1:1">
+      <c r="B44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="46" spans="1:1">
+      <c r="B45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="47" spans="1:1">
+      <c r="B46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="48" spans="1:1">
+      <c r="B47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="49" spans="1:1">
+      <c r="B48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="B49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="51" spans="1:1">
+      <c r="B50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="52" spans="1:1">
+      <c r="B51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="53" spans="1:1">
+      <c r="B52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="54" spans="1:1">
+      <c r="B53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="55" spans="1:1">
+      <c r="B54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
+      <c r="B55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="57" spans="1:1">
+      <c r="B56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="58" spans="1:1">
+      <c r="B57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="59" spans="1:1">
+      <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="60" spans="1:1">
+      <c r="B59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="61" spans="1:1">
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="62" spans="1:1">
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="63" spans="1:1">
+      <c r="B62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="64" spans="1:1">
+      <c r="B63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
       <c r="A64" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="65" spans="1:1">
+      <c r="B64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
       <c r="A65" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="66" spans="1:1">
+      <c r="B65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="67" spans="1:1">
+      <c r="B66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
       <c r="A67" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="68" spans="1:1">
+      <c r="B67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
       <c r="A68" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="69" spans="1:1">
+      <c r="B68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
       <c r="A69" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="70" spans="1:1">
+      <c r="B69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
       <c r="A70" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="71" spans="1:1">
+      <c r="B70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
       <c r="A71" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="72" spans="1:1">
+      <c r="B71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
       <c r="A72" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="73" spans="1:1">
+      <c r="B72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
       <c r="A73" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="74" spans="1:1">
+      <c r="B73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
       <c r="A74" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="75" spans="1:1">
+      <c r="B74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
       <c r="A75" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="76" spans="1:1">
+      <c r="B75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
       <c r="A76" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="77" spans="1:1">
+      <c r="B76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
       <c r="A77" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="78" spans="1:1">
+      <c r="B77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
       <c r="A78" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="79" spans="1:1">
+      <c r="B78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
       <c r="A79" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="80" spans="1:1">
+      <c r="B79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
       <c r="A80" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="81" spans="1:1">
+      <c r="B80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
       <c r="A81" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="82" spans="1:1">
+      <c r="B81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
       <c r="A82" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="83" spans="1:1">
+      <c r="B82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
       <c r="A83" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="84" spans="1:1">
+      <c r="B83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
       <c r="A84" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="85" spans="1:1">
+      <c r="B84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
       <c r="A85" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="86" spans="1:1">
+      <c r="B85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
       <c r="A86" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="87" spans="1:1">
+      <c r="B86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
       <c r="A87" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="88" spans="1:1">
+      <c r="B87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
       <c r="A88" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="89" spans="1:1">
+      <c r="B88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
       <c r="A89" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="90" spans="1:1">
+      <c r="B89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
       <c r="A90" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="91" spans="1:1">
+      <c r="B90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
       <c r="A91" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="92" spans="1:1">
+      <c r="B91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
       <c r="A92" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="93" spans="1:1">
+      <c r="B92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
       <c r="A93" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="94" spans="1:1">
+      <c r="B93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
       <c r="A94" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="95" spans="1:1">
+      <c r="B94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
       <c r="A95" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="96" spans="1:1">
+      <c r="B95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
       <c r="A96" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="97" spans="1:1">
+      <c r="B96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
       <c r="A97" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="98" spans="1:1">
+      <c r="B97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
       <c r="A98" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="99" spans="1:1">
+      <c r="B98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
       <c r="A99" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="100" spans="1:1">
+      <c r="B99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
       <c r="A100" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="101" spans="1:1">
+      <c r="B100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
       <c r="A101" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="102" spans="1:1">
-      <c r="A102" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1">
-      <c r="A103" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1">
-      <c r="A104" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1">
-      <c r="A105" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1">
-      <c r="A106" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1">
-      <c r="A107" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1">
-      <c r="A108" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1">
-      <c r="A109" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1">
-      <c r="A110" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1">
-      <c r="A111" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1">
-      <c r="A112" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1">
-      <c r="A113" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1">
-      <c r="A114" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1">
-      <c r="A115" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1">
-      <c r="A116" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1">
-      <c r="A117" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1">
-      <c r="A118" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1">
-      <c r="A119" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1">
-      <c r="A120" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1">
-      <c r="A121" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1">
-      <c r="A122" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1">
-      <c r="A123" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1">
-      <c r="A124" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1">
-      <c r="A125" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1">
-      <c r="A126" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1">
-      <c r="A127" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1">
-      <c r="A128" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1">
-      <c r="A129" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1">
-      <c r="A130" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1">
-      <c r="A131" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1">
-      <c r="A132" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1">
-      <c r="A133" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1">
-      <c r="A134" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1">
-      <c r="A135" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1">
-      <c r="A136" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1">
-      <c r="A137" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1">
-      <c r="A138" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1">
-      <c r="A139" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1">
-      <c r="A140" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1">
-      <c r="A141" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1">
-      <c r="A142" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1">
-      <c r="A143" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1">
-      <c r="A144" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1">
-      <c r="A145" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1">
-      <c r="A146" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1">
-      <c r="A147" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1">
-      <c r="A148" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1">
-      <c r="A149" t="s">
-        <v>650</v>
+      <c r="B101">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>